<commit_message>
add secondary groupings with prezresults
</commit_message>
<xml_diff>
--- a/output/groupings_for_dems_hr1296.xlsx
+++ b/output/groupings_for_dems_hr1296.xlsx
@@ -8,23 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kessler\GitHub_Kessler\congress_votes\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400F683A-BC02-40FA-BB6D-4538DB779F01}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238D96E4-B870-4CA4-9737-7AC0933E8CBE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="trump_hillary_wins" sheetId="1" r:id="rId1"/>
+    <sheet name="prezresults2016" sheetId="1" r:id="rId1"/>
     <sheet name="gdp_vs_nationalavg" sheetId="2" r:id="rId2"/>
     <sheet name="college_vs_nationalavg" sheetId="3" r:id="rId3"/>
     <sheet name="nonwhite_vs_nationalavg" sheetId="4" r:id="rId4"/>
     <sheet name="rural_morethanfifth" sheetId="5" r:id="rId5"/>
+    <sheet name="gdp_andprezresults" sheetId="6" r:id="rId6"/>
+    <sheet name="college_degree_andprezresults" sheetId="7" r:id="rId7"/>
+    <sheet name="nonwhite_pop_andprezresults" sheetId="8" r:id="rId8"/>
+    <sheet name="rural_area_andprezresults" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="13">
   <si>
     <t>p16winningparty</t>
   </si>
@@ -452,7 +456,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +531,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +606,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -677,7 +681,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,4 +840,625 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add margin of victory flag column
</commit_message>
<xml_diff>
--- a/output/groupings_for_dems_hr1296.xlsx
+++ b/output/groupings_for_dems_hr1296.xlsx
@@ -12,10 +12,12 @@
     <sheet name="college_vs_nationalavg" sheetId="3" r:id="rId3"/>
     <sheet name="nonwhite_vs_nationalavg" sheetId="4" r:id="rId4"/>
     <sheet name="rural_morethanfifth" sheetId="5" r:id="rId5"/>
-    <sheet name="gdp_andprezresults" sheetId="6" r:id="rId6"/>
-    <sheet name="college_degree_andprezresults" sheetId="7" r:id="rId7"/>
-    <sheet name="nonwhite_pop_andprezresults" sheetId="8" r:id="rId8"/>
-    <sheet name="rural_area_andprezresults" sheetId="9" r:id="rId9"/>
+    <sheet name="margin_5_or_less" sheetId="6" r:id="rId6"/>
+    <sheet name="gdp_andprezresults" sheetId="7" r:id="rId7"/>
+    <sheet name="college_degree_andprezresults" sheetId="8" r:id="rId8"/>
+    <sheet name="nonwhite_pop_andprezresults" sheetId="9" r:id="rId9"/>
+    <sheet name="rural_area_andprezresults" sheetId="10" r:id="rId10"/>
+    <sheet name="margin_5_or_less_withprez" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -447,6 +449,461 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>p16winningparty</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pct.rural.above20</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>stance</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>p16winningparty</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>margin_flag</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>stance</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5_points_or_less</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5_points_or_less</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>more_than_5_points</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>more_than_5_points</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5_points_or_less</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>5_points_or_less</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>more_than_5_points</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>more_than_5_points</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
@@ -829,7 +1286,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -838,20 +1295,15 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>p16winningparty</t>
+          <t>margin_flag</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>gdp_abovebelow_natlavg</t>
+          <t>stance</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>stance</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>n</t>
         </is>
@@ -860,161 +1312,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>5_points_or_less</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>not_sponsoring</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>2</v>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>5_points_or_less</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sponsoring</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>120</v>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>more_than_5_points</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>not_sponsoring</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>8</v>
+          <t>not_sponsoring</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>more_than_5_points</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>sponsoring</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>73</v>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>190</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>other</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>not_sponsoring</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>sponsoring</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>not_sponsoring</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>sponsoring</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>9</v>
+          <t>sponsoring</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1038,7 +1405,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pct.ed.college.all.abovebelow.natl</t>
+          <t>gdp_abovebelow_natlavg</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1069,7 +1436,7 @@
         </is>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1089,7 +1456,7 @@
         </is>
       </c>
       <c r="D3">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
@@ -1109,7 +1476,7 @@
         </is>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -1129,7 +1496,7 @@
         </is>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
@@ -1149,7 +1516,7 @@
         </is>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -1169,7 +1536,7 @@
         </is>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -1189,7 +1556,7 @@
         </is>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -1209,7 +1576,7 @@
         </is>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1600,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pct.race.nonwhite.abovebelow.natl</t>
+          <t>pct.ed.college.all.abovebelow.natl</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1264,7 +1631,7 @@
         </is>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -1284,7 +1651,7 @@
         </is>
       </c>
       <c r="D3">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
@@ -1304,7 +1671,7 @@
         </is>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -1324,7 +1691,7 @@
         </is>
       </c>
       <c r="D5">
-        <v>63</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
@@ -1344,7 +1711,7 @@
         </is>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -1364,7 +1731,7 @@
         </is>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -1384,7 +1751,7 @@
         </is>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -1404,7 +1771,7 @@
         </is>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1781,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1428,7 +1795,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>pct.rural.above20</t>
+          <t>pct.race.nonwhite.abovebelow.natl</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1459,7 +1826,7 @@
         </is>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1479,7 +1846,7 @@
         </is>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
@@ -1499,7 +1866,7 @@
         </is>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -1519,22 +1886,27 @@
         </is>
       </c>
       <c r="D5">
-        <v>172</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -1550,11 +1922,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>not_sponsoring</t>
+          <t>sponsoring</t>
         </is>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -1565,16 +1937,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -1590,61 +1962,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>not_sponsoring</t>
+          <t>sponsoring</t>
         </is>
       </c>
       <c r="D9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>sponsoring</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>not_sponsoring</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>sponsoring</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>